<commit_message>
Pip install openpyxl for our excel dataset
</commit_message>
<xml_diff>
--- a/startup_funding2019.xlsx
+++ b/startup_funding2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\AM4PEPF0002D5EE\EXCELCNV\c74f4ea9-540c-44ec-8d82-151f062e1e85\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\AM4PEPF0002D5A9\EXCELCNV\de13104f-637d-4c71-a14d-83208f66ddc1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4020775-15E4-4FB0-84B6-5CAD3DB6A74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B632887F-8091-416C-9360-AFB483FAE4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{A1B3AE3B-6F05-4FE1-93B2-23D68E1FE4B7}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{6A9E9674-02BB-4D07-A067-34AEDA623936}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -2196,7 +2196,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1B4779-8DCD-43F1-AD1B-EB2267A12647}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E86BDCA-B083-4847-B0A4-0C9AACECD026}">
   <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>